<commit_message>
update tables in excel files
</commit_message>
<xml_diff>
--- a/stability_analysis/data/cases/OperationData_IEEE_118_NREL.xlsx
+++ b/stability_analysis/data/cases/OperationData_IEEE_118_NREL.xlsx
@@ -3651,7 +3651,7 @@
         <v>561.3399000000001</v>
       </c>
       <c r="H2" t="n">
-        <v>-118.1768210526316</v>
+        <v>-561.3399000000001</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -3694,7 +3694,7 @@
         <v>31.4391</v>
       </c>
       <c r="H3" t="n">
-        <v>-6.618757894736843</v>
+        <v>-31.4391</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -3737,7 +3737,7 @@
         <v>18.5196</v>
       </c>
       <c r="H4" t="n">
-        <v>-3.898863157894737</v>
+        <v>-18.5196</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -3780,7 +3780,7 @@
         <v>33</v>
       </c>
       <c r="H5" t="n">
-        <v>-6.947368421052633</v>
+        <v>-33</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -3823,7 +3823,7 @@
         <v>100.2375</v>
       </c>
       <c r="H6" t="n">
-        <v>-21.10263157894737</v>
+        <v>-100.2375</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -3866,7 +3866,7 @@
         <v>277.6587</v>
       </c>
       <c r="H7" t="n">
-        <v>-58.45446315789474</v>
+        <v>-277.6587</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -3909,7 +3909,7 @@
         <v>53.67780000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>-11.30058947368421</v>
+        <v>-53.67780000000001</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -3952,7 +3952,7 @@
         <v>222.222</v>
       </c>
       <c r="H9" t="n">
-        <v>-46.78357894736843</v>
+        <v>-222.222</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -3995,7 +3995,7 @@
         <v>52.49640000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>-11.05187368421053</v>
+        <v>-52.49640000000001</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -4038,7 +4038,7 @@
         <v>130.4655</v>
       </c>
       <c r="H11" t="n">
-        <v>-27.46642105263158</v>
+        <v>-130.4655</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -4081,7 +4081,7 @@
         <v>542.157</v>
       </c>
       <c r="H12" t="n">
-        <v>-114.1383157894737</v>
+        <v>-542.157</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -4124,7 +4124,7 @@
         <v>204.27</v>
       </c>
       <c r="H13" t="n">
-        <v>-43.00421052631579</v>
+        <v>-204.27</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -4167,7 +4167,7 @@
         <v>589.809</v>
       </c>
       <c r="H14" t="n">
-        <v>-124.1703157894737</v>
+        <v>-589.809</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -4210,7 +4210,7 @@
         <v>518.9217</v>
       </c>
       <c r="H15" t="n">
-        <v>-109.2466736842105</v>
+        <v>-518.9217</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -4253,7 +4253,7 @@
         <v>47.751</v>
       </c>
       <c r="H16" t="n">
-        <v>-10.05284210526316</v>
+        <v>-47.751</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -4296,7 +4296,7 @@
         <v>439.0683</v>
       </c>
       <c r="H17" t="n">
-        <v>-92.43543157894739</v>
+        <v>-439.0683</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -4339,7 +4339,7 @@
         <v>307.395</v>
       </c>
       <c r="H18" t="n">
-        <v>-64.71473684210528</v>
+        <v>-307.395</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -4382,7 +4382,7 @@
         <v>30.0069</v>
       </c>
       <c r="H19" t="n">
-        <v>-6.317242105263158</v>
+        <v>-30.0069</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -4425,7 +4425,7 @@
         <v>447.579</v>
       </c>
       <c r="H20" t="n">
-        <v>-94.22715789473686</v>
+        <v>-447.579</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -4468,7 +4468,7 @@
         <v>219.219</v>
       </c>
       <c r="H21" t="n">
-        <v>-46.15136842105264</v>
+        <v>-219.219</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -4511,7 +4511,7 @@
         <v>159.0006</v>
       </c>
       <c r="H22" t="n">
-        <v>-33.47381052631579</v>
+        <v>-159.0006</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -4554,7 +4554,7 @@
         <v>55.572</v>
       </c>
       <c r="H23" t="n">
-        <v>-11.69936842105263</v>
+        <v>-55.572</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -4597,7 +4597,7 @@
         <v>49.5</v>
       </c>
       <c r="H24" t="n">
-        <v>-10.42105263157895</v>
+        <v>-49.5</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -4640,7 +4640,7 @@
         <v>42.8967</v>
       </c>
       <c r="H25" t="n">
-        <v>-9.030884210526317</v>
+        <v>-42.8967</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -4683,7 +4683,7 @@
         <v>70.95</v>
       </c>
       <c r="H26" t="n">
-        <v>-14.93684210526316</v>
+        <v>-70.95</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -4726,7 +4726,7 @@
         <v>17.82</v>
       </c>
       <c r="H27" t="n">
-        <v>-3.751578947368422</v>
+        <v>-17.82</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -4769,7 +4769,7 @@
         <v>55.11</v>
       </c>
       <c r="H28" t="n">
-        <v>-11.60210526315789</v>
+        <v>-55.11</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -4812,7 +4812,7 @@
         <v>56.991</v>
       </c>
       <c r="H29" t="n">
-        <v>-11.9981052631579</v>
+        <v>-56.991</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -4855,7 +4855,7 @@
         <v>138.93</v>
       </c>
       <c r="H30" t="n">
-        <v>-29.24842105263158</v>
+        <v>-138.93</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -4898,7 +4898,7 @@
         <v>16.8564</v>
       </c>
       <c r="H31" t="n">
-        <v>-3.548715789473685</v>
+        <v>-16.8564</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -4941,7 +4941,7 @@
         <v>134.2671</v>
       </c>
       <c r="H32" t="n">
-        <v>-28.26675789473684</v>
+        <v>-134.2671</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -4984,7 +4984,7 @@
         <v>52.27200000000001</v>
       </c>
       <c r="H33" t="n">
-        <v>-11.00463157894737</v>
+        <v>-52.27200000000001</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -5027,7 +5027,7 @@
         <v>86.17949999999999</v>
       </c>
       <c r="H34" t="n">
-        <v>-18.14305263157895</v>
+        <v>-86.17949999999999</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
         <v>109.131</v>
       </c>
       <c r="H35" t="n">
-        <v>-22.97494736842106</v>
+        <v>-109.131</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -5113,7 +5113,7 @@
         <v>106.59</v>
       </c>
       <c r="H36" t="n">
-        <v>-22.44</v>
+        <v>-106.59</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -5156,7 +5156,7 @@
         <v>82.37130000000001</v>
       </c>
       <c r="H37" t="n">
-        <v>-17.34132631578948</v>
+        <v>-82.37130000000001</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -5199,7 +5199,7 @@
         <v>92.9346</v>
       </c>
       <c r="H38" t="n">
-        <v>-19.56517894736843</v>
+        <v>-92.9346</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -5242,7 +5242,7 @@
         <v>158.763</v>
       </c>
       <c r="H39" t="n">
-        <v>-33.42378947368422</v>
+        <v>-158.763</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -5285,7 +5285,7 @@
         <v>248.2953</v>
       </c>
       <c r="H40" t="n">
-        <v>-52.27269473684211</v>
+        <v>-248.2953</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -5328,7 +5328,7 @@
         <v>33.9273</v>
       </c>
       <c r="H41" t="n">
-        <v>-7.142589473684212</v>
+        <v>-33.9273</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -5371,7 +5371,7 @@
         <v>160.941</v>
       </c>
       <c r="H42" t="n">
-        <v>-33.88231578947369</v>
+        <v>-160.941</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -5414,7 +5414,7 @@
         <v>459.1488000000001</v>
       </c>
       <c r="H43" t="n">
-        <v>-96.66290526315792</v>
+        <v>-459.1488000000001</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -5457,7 +5457,7 @@
         <v>47.5332</v>
       </c>
       <c r="H44" t="n">
-        <v>-10.00698947368421</v>
+        <v>-47.5332</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -5500,7 +5500,7 @@
         <v>154.11</v>
       </c>
       <c r="H45" t="n">
-        <v>-32.44421052631579</v>
+        <v>-154.11</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -5543,7 +5543,7 @@
         <v>83.78700000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>-17.63936842105263</v>
+        <v>-83.78700000000001</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -5586,7 +5586,7 @@
         <v>125.6409</v>
       </c>
       <c r="H47" t="n">
-        <v>-26.45071578947369</v>
+        <v>-125.6409</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -5629,7 +5629,7 @@
         <v>61.84200000000001</v>
       </c>
       <c r="H48" t="n">
-        <v>-13.01936842105263</v>
+        <v>-61.84200000000001</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -5672,7 +5672,7 @@
         <v>105.6</v>
       </c>
       <c r="H49" t="n">
-        <v>-22.23157894736843</v>
+        <v>-105.6</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -5715,7 +5715,7 @@
         <v>107.25</v>
       </c>
       <c r="H50" t="n">
-        <v>-22.57894736842105</v>
+        <v>-107.25</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -5758,7 +5758,7 @@
         <v>53.856</v>
       </c>
       <c r="H51" t="n">
-        <v>-11.3381052631579</v>
+        <v>-53.856</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -5801,7 +5801,7 @@
         <v>35.343</v>
       </c>
       <c r="H52" t="n">
-        <v>-7.440631578947371</v>
+        <v>-35.343</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
@@ -5844,7 +5844,7 @@
         <v>51.546</v>
       </c>
       <c r="H53" t="n">
-        <v>-10.85178947368421</v>
+        <v>-51.546</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -5887,7 +5887,7 @@
         <v>115.17</v>
       </c>
       <c r="H54" t="n">
-        <v>-24.24631578947369</v>
+        <v>-115.17</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
excel files with stable case result
</commit_message>
<xml_diff>
--- a/stability_analysis/data/cases/OperationData_IEEE_118_NREL.xlsx
+++ b/stability_analysis/data/cases/OperationData_IEEE_118_NREL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\miniconda3\envs\gridcal_original2\stability_analysis\stability_analysis\data\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C949E78-43F2-4979-9067-CDDB13ADC558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A859A5-4764-4612-9F7C-CBD482E92C40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26130" windowHeight="7980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26136" windowHeight="7980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loads" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Generators!$A$1:$A$54</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -802,9 +802,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -832,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -860,7 +860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -874,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -888,7 +888,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -902,7 +902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -916,7 +916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -930,7 +930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -944,7 +944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -958,7 +958,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -972,7 +972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -986,7 +986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -2103,9 +2103,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>101</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>106</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>109</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>110</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>111</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>58</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>113</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>59</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>114</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>115</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>116</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>61</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>62</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>63</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>65</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>66</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>117</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>67</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>70</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>71</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>72</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>118</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>73</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>119</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>74</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>120</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>75</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>76</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>77</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>78</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>79</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>80</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>81</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>121</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>82</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>83</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>84</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>85</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>86</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>87</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>88</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>89</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>90</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>91</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>92</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>122</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>93</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>94</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>95</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>96</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>97</v>
       </c>
@@ -3067,12 +3067,12 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="H2" sqref="H2:H54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>125</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -3136,7 +3136,8 @@
         <v>47.750999999999998</v>
       </c>
       <c r="H2">
-        <v>-10.05284210526316</v>
+        <f>-G2</f>
+        <v>-47.750999999999998</v>
       </c>
       <c r="I2" t="s">
         <v>5</v>
@@ -3154,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6</v>
       </c>
@@ -3177,7 +3178,8 @@
         <v>55.572000000000003</v>
       </c>
       <c r="H3">
-        <v>-11.699368421052631</v>
+        <f t="shared" ref="H3:H54" si="0">-G3</f>
+        <v>-55.572000000000003</v>
       </c>
       <c r="I3" t="s">
         <v>5</v>
@@ -3195,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -3218,7 +3220,8 @@
         <v>49.5</v>
       </c>
       <c r="H4">
-        <v>-10.42105263157895</v>
+        <f t="shared" si="0"/>
+        <v>-49.5</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
@@ -3236,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10</v>
       </c>
@@ -3259,7 +3262,8 @@
         <v>518.92169999999999</v>
       </c>
       <c r="H5">
-        <v>-109.24667368421051</v>
+        <f t="shared" si="0"/>
+        <v>-518.92169999999999</v>
       </c>
       <c r="I5" t="s">
         <v>5</v>
@@ -3277,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>12</v>
       </c>
@@ -3300,7 +3304,8 @@
         <v>561.33990000000006</v>
       </c>
       <c r="H6">
-        <v>-118.1768210526316</v>
+        <f t="shared" si="0"/>
+        <v>-561.33990000000006</v>
       </c>
       <c r="I6" t="s">
         <v>5</v>
@@ -3318,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>15</v>
       </c>
@@ -3341,7 +3346,8 @@
         <v>47.533200000000001</v>
       </c>
       <c r="H7">
-        <v>-10.006989473684211</v>
+        <f t="shared" si="0"/>
+        <v>-47.533200000000001</v>
       </c>
       <c r="I7" t="s">
         <v>5</v>
@@ -3359,7 +3365,7 @@
         <v>30.324210526315792</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>18</v>
       </c>
@@ -3382,7 +3388,8 @@
         <v>159.00059999999999</v>
       </c>
       <c r="H8">
-        <v>-33.473810526315788</v>
+        <f t="shared" si="0"/>
+        <v>-159.00059999999999</v>
       </c>
       <c r="I8" t="s">
         <v>5</v>
@@ -3400,7 +3407,7 @@
         <v>39.056842105263158</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>19</v>
       </c>
@@ -3423,7 +3430,8 @@
         <v>61.842000000000013</v>
       </c>
       <c r="H9">
-        <v>-13.019368421052629</v>
+        <f t="shared" si="0"/>
+        <v>-61.842000000000013</v>
       </c>
       <c r="I9" t="s">
         <v>5</v>
@@ -3441,7 +3449,7 @@
         <v>26.273684210526319</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>24</v>
       </c>
@@ -3464,7 +3472,8 @@
         <v>53.856000000000002</v>
       </c>
       <c r="H10">
-        <v>-11.3381052631579</v>
+        <f t="shared" si="0"/>
+        <v>-53.856000000000002</v>
       </c>
       <c r="I10" t="s">
         <v>5</v>
@@ -3482,7 +3491,7 @@
         <v>13.81052631578947</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>25</v>
       </c>
@@ -3505,7 +3514,8 @@
         <v>542.15700000000004</v>
       </c>
       <c r="H11">
-        <v>-114.13831578947369</v>
+        <f t="shared" si="0"/>
+        <v>-542.15700000000004</v>
       </c>
       <c r="I11" t="s">
         <v>5</v>
@@ -3523,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>26</v>
       </c>
@@ -3546,7 +3556,8 @@
         <v>589.80899999999997</v>
       </c>
       <c r="H12">
-        <v>-124.1703157894737</v>
+        <f t="shared" si="0"/>
+        <v>-589.80899999999997</v>
       </c>
       <c r="I12" t="s">
         <v>5</v>
@@ -3564,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>27</v>
       </c>
@@ -3587,7 +3598,8 @@
         <v>35.343000000000004</v>
       </c>
       <c r="H13">
-        <v>-7.4406315789473707</v>
+        <f t="shared" si="0"/>
+        <v>-35.343000000000004</v>
       </c>
       <c r="I13" t="s">
         <v>5</v>
@@ -3605,7 +3617,7 @@
         <v>22.547368421052639</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>31</v>
       </c>
@@ -3628,7 +3640,8 @@
         <v>51.545999999999999</v>
       </c>
       <c r="H14">
-        <v>-10.85178947368421</v>
+        <f t="shared" si="0"/>
+        <v>-51.545999999999999</v>
       </c>
       <c r="I14" t="s">
         <v>5</v>
@@ -3646,7 +3659,7 @@
         <v>32.88421052631579</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>32</v>
       </c>
@@ -3669,7 +3682,8 @@
         <v>248.2953</v>
       </c>
       <c r="H15">
-        <v>-52.272694736842112</v>
+        <f t="shared" si="0"/>
+        <v>-248.2953</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
@@ -3687,7 +3701,7 @@
         <v>158.23368421052629</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>34</v>
       </c>
@@ -3710,7 +3724,8 @@
         <v>18.519600000000001</v>
       </c>
       <c r="H16">
-        <v>-3.8988631578947368</v>
+        <f t="shared" si="0"/>
+        <v>-18.519600000000001</v>
       </c>
       <c r="I16" t="s">
         <v>30</v>
@@ -3728,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>36</v>
       </c>
@@ -3751,7 +3766,8 @@
         <v>53.677800000000012</v>
       </c>
       <c r="H17">
-        <v>-11.300589473684211</v>
+        <f t="shared" si="0"/>
+        <v>-53.677800000000012</v>
       </c>
       <c r="I17" t="s">
         <v>30</v>
@@ -3769,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>40</v>
       </c>
@@ -3792,7 +3808,8 @@
         <v>17.82</v>
       </c>
       <c r="H18">
-        <v>-3.7515789473684218</v>
+        <f t="shared" si="0"/>
+        <v>-17.82</v>
       </c>
       <c r="I18" t="s">
         <v>30</v>
@@ -3810,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>42</v>
       </c>
@@ -3833,7 +3850,8 @@
         <v>16.856400000000001</v>
       </c>
       <c r="H19">
-        <v>-3.5487157894736852</v>
+        <f t="shared" si="0"/>
+        <v>-16.856400000000001</v>
       </c>
       <c r="I19" t="s">
         <v>30</v>
@@ -3851,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>46</v>
       </c>
@@ -3874,7 +3892,8 @@
         <v>52.496400000000008</v>
       </c>
       <c r="H20">
-        <v>-11.051873684210531</v>
+        <f t="shared" si="0"/>
+        <v>-52.496400000000008</v>
       </c>
       <c r="I20" t="s">
         <v>30</v>
@@ -3892,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>49</v>
       </c>
@@ -3915,7 +3934,8 @@
         <v>130.46549999999999</v>
       </c>
       <c r="H21">
-        <v>-27.466421052631581</v>
+        <f t="shared" si="0"/>
+        <v>-130.46549999999999</v>
       </c>
       <c r="I21" t="s">
         <v>30</v>
@@ -3933,7 +3953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>54</v>
       </c>
@@ -3956,7 +3976,8 @@
         <v>134.2671</v>
       </c>
       <c r="H22">
-        <v>-28.266757894736841</v>
+        <f t="shared" si="0"/>
+        <v>-134.2671</v>
       </c>
       <c r="I22" t="s">
         <v>30</v>
@@ -3974,7 +3995,7 @@
         <v>55.677894736842113</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>55</v>
       </c>
@@ -3997,7 +4018,8 @@
         <v>56.991</v>
       </c>
       <c r="H23">
-        <v>-11.9981052631579</v>
+        <f t="shared" si="0"/>
+        <v>-56.991</v>
       </c>
       <c r="I23" t="s">
         <v>30</v>
@@ -4015,7 +4037,7 @@
         <v>6.3157894736842124</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>56</v>
       </c>
@@ -4038,7 +4060,8 @@
         <v>52.272000000000013</v>
       </c>
       <c r="H24">
-        <v>-11.00463157894737</v>
+        <f t="shared" si="0"/>
+        <v>-52.272000000000013</v>
       </c>
       <c r="I24" t="s">
         <v>30</v>
@@ -4056,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>59</v>
       </c>
@@ -4079,7 +4102,8 @@
         <v>109.131</v>
       </c>
       <c r="H25">
-        <v>-22.974947368421059</v>
+        <f t="shared" si="0"/>
+        <v>-109.131</v>
       </c>
       <c r="I25" t="s">
         <v>30</v>
@@ -4097,7 +4121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>61</v>
       </c>
@@ -4120,7 +4144,8 @@
         <v>106.59</v>
       </c>
       <c r="H26">
-        <v>-22.44</v>
+        <f t="shared" si="0"/>
+        <v>-106.59</v>
       </c>
       <c r="I26" t="s">
         <v>30</v>
@@ -4138,7 +4163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>62</v>
       </c>
@@ -4161,7 +4186,8 @@
         <v>55.11</v>
       </c>
       <c r="H27">
-        <v>-11.60210526315789</v>
+        <f t="shared" si="0"/>
+        <v>-55.11</v>
       </c>
       <c r="I27" t="s">
         <v>30</v>
@@ -4179,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>65</v>
       </c>
@@ -4202,7 +4228,8 @@
         <v>219.21899999999999</v>
       </c>
       <c r="H28">
-        <v>-46.151368421052638</v>
+        <f t="shared" si="0"/>
+        <v>-219.21899999999999</v>
       </c>
       <c r="I28" t="s">
         <v>30</v>
@@ -4220,7 +4247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>66</v>
       </c>
@@ -4243,7 +4270,8 @@
         <v>222.22200000000001</v>
       </c>
       <c r="H29">
-        <v>-46.783578947368433</v>
+        <f t="shared" si="0"/>
+        <v>-222.22200000000001</v>
       </c>
       <c r="I29" t="s">
         <v>30</v>
@@ -4261,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>69</v>
       </c>
@@ -4284,7 +4312,8 @@
         <v>160.941</v>
       </c>
       <c r="H30">
-        <v>-33.882315789473687</v>
+        <f t="shared" si="0"/>
+        <v>-160.941</v>
       </c>
       <c r="I30" t="s">
         <v>30</v>
@@ -4302,7 +4331,7 @@
         <v>26.294736842105269</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>70</v>
       </c>
@@ -4325,7 +4354,8 @@
         <v>105.6</v>
       </c>
       <c r="H31">
-        <v>-22.23157894736843</v>
+        <f t="shared" si="0"/>
+        <v>-105.6</v>
       </c>
       <c r="I31" t="s">
         <v>5</v>
@@ -4343,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>72</v>
       </c>
@@ -4366,7 +4396,8 @@
         <v>107.25</v>
       </c>
       <c r="H32">
-        <v>-22.578947368421051</v>
+        <f t="shared" si="0"/>
+        <v>-107.25</v>
       </c>
       <c r="I32" t="s">
         <v>5</v>
@@ -4384,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>74</v>
       </c>
@@ -4407,7 +4438,8 @@
         <v>33</v>
       </c>
       <c r="H33">
-        <v>-6.9473684210526327</v>
+        <f t="shared" si="0"/>
+        <v>-33</v>
       </c>
       <c r="I33" t="s">
         <v>5</v>
@@ -4425,7 +4457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>76</v>
       </c>
@@ -4448,7 +4480,8 @@
         <v>86.17949999999999</v>
       </c>
       <c r="H34">
-        <v>-18.14305263157895</v>
+        <f t="shared" si="0"/>
+        <v>-86.17949999999999</v>
       </c>
       <c r="I34" t="s">
         <v>30</v>
@@ -4466,7 +4499,7 @@
         <v>5.2631578947368416</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>77</v>
       </c>
@@ -4489,7 +4522,8 @@
         <v>82.371300000000005</v>
       </c>
       <c r="H35">
-        <v>-17.34132631578948</v>
+        <f t="shared" si="0"/>
+        <v>-82.371300000000005</v>
       </c>
       <c r="I35" t="s">
         <v>30</v>
@@ -4507,7 +4541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>80</v>
       </c>
@@ -4530,7 +4564,8 @@
         <v>158.76300000000001</v>
       </c>
       <c r="H36">
-        <v>-33.423789473684216</v>
+        <f t="shared" si="0"/>
+        <v>-158.76300000000001</v>
       </c>
       <c r="I36" t="s">
         <v>30</v>
@@ -4548,7 +4583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>82</v>
       </c>
@@ -4571,7 +4606,8 @@
         <v>115.17</v>
       </c>
       <c r="H37">
-        <v>-24.246315789473691</v>
+        <f t="shared" si="0"/>
+        <v>-115.17</v>
       </c>
       <c r="I37" t="s">
         <v>68</v>
@@ -4589,7 +4625,7 @@
         <v>73.473684210526329</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>85</v>
       </c>
@@ -4612,7 +4648,8 @@
         <v>42.896700000000003</v>
       </c>
       <c r="H38">
-        <v>-9.0308842105263167</v>
+        <f t="shared" si="0"/>
+        <v>-42.896700000000003</v>
       </c>
       <c r="I38" t="s">
         <v>68</v>
@@ -4630,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>87</v>
       </c>
@@ -4653,7 +4690,8 @@
         <v>447.57900000000001</v>
       </c>
       <c r="H39">
-        <v>-94.227157894736862</v>
+        <f t="shared" si="0"/>
+        <v>-447.57900000000001</v>
       </c>
       <c r="I39" t="s">
         <v>68</v>
@@ -4671,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>89</v>
       </c>
@@ -4694,7 +4732,8 @@
         <v>307.39499999999998</v>
       </c>
       <c r="H40">
-        <v>-64.714736842105282</v>
+        <f t="shared" si="0"/>
+        <v>-307.39499999999998</v>
       </c>
       <c r="I40" t="s">
         <v>68</v>
@@ -4712,7 +4751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>90</v>
       </c>
@@ -4735,7 +4774,8 @@
         <v>30.006900000000002</v>
       </c>
       <c r="H41">
-        <v>-6.3172421052631584</v>
+        <f t="shared" si="0"/>
+        <v>-30.006900000000002</v>
       </c>
       <c r="I41" t="s">
         <v>68</v>
@@ -4753,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>91</v>
       </c>
@@ -4776,7 +4816,8 @@
         <v>70.95</v>
       </c>
       <c r="H42">
-        <v>-14.93684210526316</v>
+        <f t="shared" si="0"/>
+        <v>-70.95</v>
       </c>
       <c r="I42" t="s">
         <v>68</v>
@@ -4794,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>92</v>
       </c>
@@ -4817,7 +4858,8 @@
         <v>459.14880000000011</v>
       </c>
       <c r="H43">
-        <v>-96.662905263157924</v>
+        <f t="shared" si="0"/>
+        <v>-459.14880000000011</v>
       </c>
       <c r="I43" t="s">
         <v>68</v>
@@ -4835,7 +4877,7 @@
         <v>109.31789473684211</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>99</v>
       </c>
@@ -4858,7 +4900,8 @@
         <v>92.934600000000003</v>
       </c>
       <c r="H44">
-        <v>-19.56517894736843</v>
+        <f t="shared" si="0"/>
+        <v>-92.934600000000003</v>
       </c>
       <c r="I44" t="s">
         <v>30</v>
@@ -4876,7 +4919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>100</v>
       </c>
@@ -4899,7 +4942,8 @@
         <v>439.06830000000002</v>
       </c>
       <c r="H45">
-        <v>-92.435431578947387</v>
+        <f t="shared" si="0"/>
+        <v>-439.06830000000002</v>
       </c>
       <c r="I45" t="s">
         <v>68</v>
@@ -4917,7 +4961,7 @@
         <v>106.3136842105263</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>103</v>
       </c>
@@ -4940,7 +4984,8 @@
         <v>31.4391</v>
       </c>
       <c r="H46">
-        <v>-6.6187578947368433</v>
+        <f t="shared" si="0"/>
+        <v>-31.4391</v>
       </c>
       <c r="I46" t="s">
         <v>68</v>
@@ -4958,7 +5003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>104</v>
       </c>
@@ -4981,7 +5026,8 @@
         <v>154.11000000000001</v>
       </c>
       <c r="H47">
-        <v>-32.444210526315793</v>
+        <f t="shared" si="0"/>
+        <v>-154.11000000000001</v>
       </c>
       <c r="I47" t="s">
         <v>68</v>
@@ -4999,7 +5045,7 @@
         <v>98.31578947368422</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>105</v>
       </c>
@@ -5022,7 +5068,8 @@
         <v>125.6409</v>
       </c>
       <c r="H48">
-        <v>-26.450715789473691</v>
+        <f t="shared" si="0"/>
+        <v>-125.6409</v>
       </c>
       <c r="I48" t="s">
         <v>68</v>
@@ -5040,7 +5087,7 @@
         <v>57.785263157894747</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>107</v>
       </c>
@@ -5063,7 +5110,8 @@
         <v>277.65870000000001</v>
       </c>
       <c r="H49">
-        <v>-58.454463157894743</v>
+        <f t="shared" si="0"/>
+        <v>-277.65870000000001</v>
       </c>
       <c r="I49" t="s">
         <v>68</v>
@@ -5081,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>110</v>
       </c>
@@ -5104,7 +5152,8 @@
         <v>83.787000000000006</v>
       </c>
       <c r="H50">
-        <v>-17.63936842105263</v>
+        <f t="shared" si="0"/>
+        <v>-83.787000000000006</v>
       </c>
       <c r="I50" t="s">
         <v>68</v>
@@ -5122,7 +5171,7 @@
         <v>53.452631578947383</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>111</v>
       </c>
@@ -5145,7 +5194,8 @@
         <v>138.93</v>
       </c>
       <c r="H51">
-        <v>-29.248421052631581</v>
+        <f t="shared" si="0"/>
+        <v>-138.93</v>
       </c>
       <c r="I51" t="s">
         <v>68</v>
@@ -5163,7 +5213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>112</v>
       </c>
@@ -5186,7 +5236,8 @@
         <v>100.2375</v>
       </c>
       <c r="H52">
-        <v>-21.102631578947371</v>
+        <f t="shared" si="0"/>
+        <v>-100.2375</v>
       </c>
       <c r="I52" t="s">
         <v>68</v>
@@ -5204,7 +5255,7 @@
         <v>37.010526315789477</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>113</v>
       </c>
@@ -5227,7 +5278,8 @@
         <v>204.27</v>
       </c>
       <c r="H53">
-        <v>-43.004210526315788</v>
+        <f t="shared" si="0"/>
+        <v>-204.27</v>
       </c>
       <c r="I53" t="s">
         <v>5</v>
@@ -5245,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>116</v>
       </c>
@@ -5268,7 +5320,8 @@
         <v>33.927300000000002</v>
       </c>
       <c r="H54">
-        <v>-7.1425894736842119</v>
+        <f t="shared" si="0"/>
+        <v>-33.927300000000002</v>
       </c>
       <c r="I54" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
fix Qmin in OperationData118NREL
</commit_message>
<xml_diff>
--- a/stability_analysis/data/cases/OperationData_IEEE_118_NREL.xlsx
+++ b/stability_analysis/data/cases/OperationData_IEEE_118_NREL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\miniconda3\envs\gridcal_original2\stability_analysis\stability_analysis\data\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C949E78-43F2-4979-9067-CDDB13ADC558}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D8CF36-E408-4911-A373-2AFE6965E56E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26130" windowHeight="7980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Generators!$A$1:$A$54</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -3067,7 +3067,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="H2" sqref="H2:H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3136,8 @@
         <v>47.750999999999998</v>
       </c>
       <c r="H2">
-        <v>-10.05284210526316</v>
+        <f>-G2</f>
+        <v>-47.750999999999998</v>
       </c>
       <c r="I2" t="s">
         <v>5</v>
@@ -3177,7 +3178,8 @@
         <v>55.572000000000003</v>
       </c>
       <c r="H3">
-        <v>-11.699368421052631</v>
+        <f t="shared" ref="H3:H54" si="0">-G3</f>
+        <v>-55.572000000000003</v>
       </c>
       <c r="I3" t="s">
         <v>5</v>
@@ -3218,7 +3220,8 @@
         <v>49.5</v>
       </c>
       <c r="H4">
-        <v>-10.42105263157895</v>
+        <f t="shared" si="0"/>
+        <v>-49.5</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
@@ -3259,7 +3262,8 @@
         <v>518.92169999999999</v>
       </c>
       <c r="H5">
-        <v>-109.24667368421051</v>
+        <f t="shared" si="0"/>
+        <v>-518.92169999999999</v>
       </c>
       <c r="I5" t="s">
         <v>5</v>
@@ -3300,7 +3304,8 @@
         <v>561.33990000000006</v>
       </c>
       <c r="H6">
-        <v>-118.1768210526316</v>
+        <f t="shared" si="0"/>
+        <v>-561.33990000000006</v>
       </c>
       <c r="I6" t="s">
         <v>5</v>
@@ -3341,7 +3346,8 @@
         <v>47.533200000000001</v>
       </c>
       <c r="H7">
-        <v>-10.006989473684211</v>
+        <f t="shared" si="0"/>
+        <v>-47.533200000000001</v>
       </c>
       <c r="I7" t="s">
         <v>5</v>
@@ -3382,7 +3388,8 @@
         <v>159.00059999999999</v>
       </c>
       <c r="H8">
-        <v>-33.473810526315788</v>
+        <f t="shared" si="0"/>
+        <v>-159.00059999999999</v>
       </c>
       <c r="I8" t="s">
         <v>5</v>
@@ -3423,7 +3430,8 @@
         <v>61.842000000000013</v>
       </c>
       <c r="H9">
-        <v>-13.019368421052629</v>
+        <f t="shared" si="0"/>
+        <v>-61.842000000000013</v>
       </c>
       <c r="I9" t="s">
         <v>5</v>
@@ -3464,7 +3472,8 @@
         <v>53.856000000000002</v>
       </c>
       <c r="H10">
-        <v>-11.3381052631579</v>
+        <f t="shared" si="0"/>
+        <v>-53.856000000000002</v>
       </c>
       <c r="I10" t="s">
         <v>5</v>
@@ -3505,7 +3514,8 @@
         <v>542.15700000000004</v>
       </c>
       <c r="H11">
-        <v>-114.13831578947369</v>
+        <f t="shared" si="0"/>
+        <v>-542.15700000000004</v>
       </c>
       <c r="I11" t="s">
         <v>5</v>
@@ -3546,7 +3556,8 @@
         <v>589.80899999999997</v>
       </c>
       <c r="H12">
-        <v>-124.1703157894737</v>
+        <f t="shared" si="0"/>
+        <v>-589.80899999999997</v>
       </c>
       <c r="I12" t="s">
         <v>5</v>
@@ -3587,7 +3598,8 @@
         <v>35.343000000000004</v>
       </c>
       <c r="H13">
-        <v>-7.4406315789473707</v>
+        <f t="shared" si="0"/>
+        <v>-35.343000000000004</v>
       </c>
       <c r="I13" t="s">
         <v>5</v>
@@ -3628,7 +3640,8 @@
         <v>51.545999999999999</v>
       </c>
       <c r="H14">
-        <v>-10.85178947368421</v>
+        <f t="shared" si="0"/>
+        <v>-51.545999999999999</v>
       </c>
       <c r="I14" t="s">
         <v>5</v>
@@ -3669,7 +3682,8 @@
         <v>248.2953</v>
       </c>
       <c r="H15">
-        <v>-52.272694736842112</v>
+        <f t="shared" si="0"/>
+        <v>-248.2953</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
@@ -3710,7 +3724,8 @@
         <v>18.519600000000001</v>
       </c>
       <c r="H16">
-        <v>-3.8988631578947368</v>
+        <f t="shared" si="0"/>
+        <v>-18.519600000000001</v>
       </c>
       <c r="I16" t="s">
         <v>30</v>
@@ -3751,7 +3766,8 @@
         <v>53.677800000000012</v>
       </c>
       <c r="H17">
-        <v>-11.300589473684211</v>
+        <f t="shared" si="0"/>
+        <v>-53.677800000000012</v>
       </c>
       <c r="I17" t="s">
         <v>30</v>
@@ -3792,7 +3808,8 @@
         <v>17.82</v>
       </c>
       <c r="H18">
-        <v>-3.7515789473684218</v>
+        <f t="shared" si="0"/>
+        <v>-17.82</v>
       </c>
       <c r="I18" t="s">
         <v>30</v>
@@ -3833,7 +3850,8 @@
         <v>16.856400000000001</v>
       </c>
       <c r="H19">
-        <v>-3.5487157894736852</v>
+        <f t="shared" si="0"/>
+        <v>-16.856400000000001</v>
       </c>
       <c r="I19" t="s">
         <v>30</v>
@@ -3874,7 +3892,8 @@
         <v>52.496400000000008</v>
       </c>
       <c r="H20">
-        <v>-11.051873684210531</v>
+        <f t="shared" si="0"/>
+        <v>-52.496400000000008</v>
       </c>
       <c r="I20" t="s">
         <v>30</v>
@@ -3915,7 +3934,8 @@
         <v>130.46549999999999</v>
       </c>
       <c r="H21">
-        <v>-27.466421052631581</v>
+        <f t="shared" si="0"/>
+        <v>-130.46549999999999</v>
       </c>
       <c r="I21" t="s">
         <v>30</v>
@@ -3956,7 +3976,8 @@
         <v>134.2671</v>
       </c>
       <c r="H22">
-        <v>-28.266757894736841</v>
+        <f t="shared" si="0"/>
+        <v>-134.2671</v>
       </c>
       <c r="I22" t="s">
         <v>30</v>
@@ -3997,7 +4018,8 @@
         <v>56.991</v>
       </c>
       <c r="H23">
-        <v>-11.9981052631579</v>
+        <f t="shared" si="0"/>
+        <v>-56.991</v>
       </c>
       <c r="I23" t="s">
         <v>30</v>
@@ -4038,7 +4060,8 @@
         <v>52.272000000000013</v>
       </c>
       <c r="H24">
-        <v>-11.00463157894737</v>
+        <f t="shared" si="0"/>
+        <v>-52.272000000000013</v>
       </c>
       <c r="I24" t="s">
         <v>30</v>
@@ -4079,7 +4102,8 @@
         <v>109.131</v>
       </c>
       <c r="H25">
-        <v>-22.974947368421059</v>
+        <f t="shared" si="0"/>
+        <v>-109.131</v>
       </c>
       <c r="I25" t="s">
         <v>30</v>
@@ -4120,7 +4144,8 @@
         <v>106.59</v>
       </c>
       <c r="H26">
-        <v>-22.44</v>
+        <f t="shared" si="0"/>
+        <v>-106.59</v>
       </c>
       <c r="I26" t="s">
         <v>30</v>
@@ -4161,7 +4186,8 @@
         <v>55.11</v>
       </c>
       <c r="H27">
-        <v>-11.60210526315789</v>
+        <f t="shared" si="0"/>
+        <v>-55.11</v>
       </c>
       <c r="I27" t="s">
         <v>30</v>
@@ -4202,7 +4228,8 @@
         <v>219.21899999999999</v>
       </c>
       <c r="H28">
-        <v>-46.151368421052638</v>
+        <f t="shared" si="0"/>
+        <v>-219.21899999999999</v>
       </c>
       <c r="I28" t="s">
         <v>30</v>
@@ -4243,7 +4270,8 @@
         <v>222.22200000000001</v>
       </c>
       <c r="H29">
-        <v>-46.783578947368433</v>
+        <f t="shared" si="0"/>
+        <v>-222.22200000000001</v>
       </c>
       <c r="I29" t="s">
         <v>30</v>
@@ -4284,7 +4312,8 @@
         <v>160.941</v>
       </c>
       <c r="H30">
-        <v>-33.882315789473687</v>
+        <f t="shared" si="0"/>
+        <v>-160.941</v>
       </c>
       <c r="I30" t="s">
         <v>30</v>
@@ -4325,7 +4354,8 @@
         <v>105.6</v>
       </c>
       <c r="H31">
-        <v>-22.23157894736843</v>
+        <f t="shared" si="0"/>
+        <v>-105.6</v>
       </c>
       <c r="I31" t="s">
         <v>5</v>
@@ -4366,7 +4396,8 @@
         <v>107.25</v>
       </c>
       <c r="H32">
-        <v>-22.578947368421051</v>
+        <f t="shared" si="0"/>
+        <v>-107.25</v>
       </c>
       <c r="I32" t="s">
         <v>5</v>
@@ -4407,7 +4438,8 @@
         <v>33</v>
       </c>
       <c r="H33">
-        <v>-6.9473684210526327</v>
+        <f t="shared" si="0"/>
+        <v>-33</v>
       </c>
       <c r="I33" t="s">
         <v>5</v>
@@ -4448,7 +4480,8 @@
         <v>86.17949999999999</v>
       </c>
       <c r="H34">
-        <v>-18.14305263157895</v>
+        <f t="shared" si="0"/>
+        <v>-86.17949999999999</v>
       </c>
       <c r="I34" t="s">
         <v>30</v>
@@ -4489,7 +4522,8 @@
         <v>82.371300000000005</v>
       </c>
       <c r="H35">
-        <v>-17.34132631578948</v>
+        <f t="shared" si="0"/>
+        <v>-82.371300000000005</v>
       </c>
       <c r="I35" t="s">
         <v>30</v>
@@ -4530,7 +4564,8 @@
         <v>158.76300000000001</v>
       </c>
       <c r="H36">
-        <v>-33.423789473684216</v>
+        <f t="shared" si="0"/>
+        <v>-158.76300000000001</v>
       </c>
       <c r="I36" t="s">
         <v>30</v>
@@ -4571,7 +4606,8 @@
         <v>115.17</v>
       </c>
       <c r="H37">
-        <v>-24.246315789473691</v>
+        <f t="shared" si="0"/>
+        <v>-115.17</v>
       </c>
       <c r="I37" t="s">
         <v>68</v>
@@ -4612,7 +4648,8 @@
         <v>42.896700000000003</v>
       </c>
       <c r="H38">
-        <v>-9.0308842105263167</v>
+        <f t="shared" si="0"/>
+        <v>-42.896700000000003</v>
       </c>
       <c r="I38" t="s">
         <v>68</v>
@@ -4653,7 +4690,8 @@
         <v>447.57900000000001</v>
       </c>
       <c r="H39">
-        <v>-94.227157894736862</v>
+        <f t="shared" si="0"/>
+        <v>-447.57900000000001</v>
       </c>
       <c r="I39" t="s">
         <v>68</v>
@@ -4694,7 +4732,8 @@
         <v>307.39499999999998</v>
       </c>
       <c r="H40">
-        <v>-64.714736842105282</v>
+        <f t="shared" si="0"/>
+        <v>-307.39499999999998</v>
       </c>
       <c r="I40" t="s">
         <v>68</v>
@@ -4735,7 +4774,8 @@
         <v>30.006900000000002</v>
       </c>
       <c r="H41">
-        <v>-6.3172421052631584</v>
+        <f t="shared" si="0"/>
+        <v>-30.006900000000002</v>
       </c>
       <c r="I41" t="s">
         <v>68</v>
@@ -4776,7 +4816,8 @@
         <v>70.95</v>
       </c>
       <c r="H42">
-        <v>-14.93684210526316</v>
+        <f t="shared" si="0"/>
+        <v>-70.95</v>
       </c>
       <c r="I42" t="s">
         <v>68</v>
@@ -4817,7 +4858,8 @@
         <v>459.14880000000011</v>
       </c>
       <c r="H43">
-        <v>-96.662905263157924</v>
+        <f t="shared" si="0"/>
+        <v>-459.14880000000011</v>
       </c>
       <c r="I43" t="s">
         <v>68</v>
@@ -4858,7 +4900,8 @@
         <v>92.934600000000003</v>
       </c>
       <c r="H44">
-        <v>-19.56517894736843</v>
+        <f t="shared" si="0"/>
+        <v>-92.934600000000003</v>
       </c>
       <c r="I44" t="s">
         <v>30</v>
@@ -4899,7 +4942,8 @@
         <v>439.06830000000002</v>
       </c>
       <c r="H45">
-        <v>-92.435431578947387</v>
+        <f t="shared" si="0"/>
+        <v>-439.06830000000002</v>
       </c>
       <c r="I45" t="s">
         <v>68</v>
@@ -4940,7 +4984,8 @@
         <v>31.4391</v>
       </c>
       <c r="H46">
-        <v>-6.6187578947368433</v>
+        <f t="shared" si="0"/>
+        <v>-31.4391</v>
       </c>
       <c r="I46" t="s">
         <v>68</v>
@@ -4981,7 +5026,8 @@
         <v>154.11000000000001</v>
       </c>
       <c r="H47">
-        <v>-32.444210526315793</v>
+        <f t="shared" si="0"/>
+        <v>-154.11000000000001</v>
       </c>
       <c r="I47" t="s">
         <v>68</v>
@@ -5022,7 +5068,8 @@
         <v>125.6409</v>
       </c>
       <c r="H48">
-        <v>-26.450715789473691</v>
+        <f t="shared" si="0"/>
+        <v>-125.6409</v>
       </c>
       <c r="I48" t="s">
         <v>68</v>
@@ -5063,7 +5110,8 @@
         <v>277.65870000000001</v>
       </c>
       <c r="H49">
-        <v>-58.454463157894743</v>
+        <f t="shared" si="0"/>
+        <v>-277.65870000000001</v>
       </c>
       <c r="I49" t="s">
         <v>68</v>
@@ -5104,7 +5152,8 @@
         <v>83.787000000000006</v>
       </c>
       <c r="H50">
-        <v>-17.63936842105263</v>
+        <f t="shared" si="0"/>
+        <v>-83.787000000000006</v>
       </c>
       <c r="I50" t="s">
         <v>68</v>
@@ -5145,7 +5194,8 @@
         <v>138.93</v>
       </c>
       <c r="H51">
-        <v>-29.248421052631581</v>
+        <f t="shared" si="0"/>
+        <v>-138.93</v>
       </c>
       <c r="I51" t="s">
         <v>68</v>
@@ -5186,7 +5236,8 @@
         <v>100.2375</v>
       </c>
       <c r="H52">
-        <v>-21.102631578947371</v>
+        <f t="shared" si="0"/>
+        <v>-100.2375</v>
       </c>
       <c r="I52" t="s">
         <v>68</v>
@@ -5227,7 +5278,8 @@
         <v>204.27</v>
       </c>
       <c r="H53">
-        <v>-43.004210526315788</v>
+        <f t="shared" si="0"/>
+        <v>-204.27</v>
       </c>
       <c r="I53" t="s">
         <v>5</v>
@@ -5268,7 +5320,8 @@
         <v>33.927300000000002</v>
       </c>
       <c r="H54">
-        <v>-7.1425894736842119</v>
+        <f t="shared" si="0"/>
+        <v>-33.927300000000002</v>
       </c>
       <c r="I54" t="s">
         <v>30</v>

</xml_diff>